<commit_message>
Connect To Camera Through USB Port and create Reload features
</commit_message>
<xml_diff>
--- a/ObjectDetection/ObjectDectecionWithOpenCV/TestData/test.xlsx
+++ b/ObjectDetection/ObjectDectecionWithOpenCV/TestData/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
+    <workbookView minimized="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -561,45 +562,136 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G7"/>
+  <dimension ref="B2:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G3">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>0</v>
       </c>
+      <c r="E4">
+        <v>63</v>
+      </c>
       <c r="G4">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G5">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>90</v>
+      </c>
       <c r="G6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>157</v>
+      </c>
+      <c r="E2">
+        <v>34</v>
+      </c>
+      <c r="G2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>62</v>
+      </c>
+      <c r="E4">
+        <v>157</v>
+      </c>
+      <c r="J4">
+        <v>56</v>
+      </c>
+      <c r="L4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>34</v>
+      </c>
+      <c r="H6">
+        <v>94</v>
+      </c>
+      <c r="L6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>157</v>
+      </c>
+      <c r="K7">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimize and refactor the source code
</commit_message>
<xml_diff>
--- a/ObjectDetection/ObjectDectecionWithOpenCV/TestData/test.xlsx
+++ b/ObjectDetection/ObjectDectecionWithOpenCV/TestData/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="7"/>
+    <workbookView minimized="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -702,23 +703,26 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F8"/>
+  <dimension ref="B1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>129</v>
       </c>
       <c r="E1">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>100</v>
       </c>
@@ -726,7 +730,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>129</v>
       </c>
@@ -734,14 +738,113 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D6">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>63</v>
+      </c>
+      <c r="D2">
+        <v>63</v>
+      </c>
+      <c r="E2">
+        <v>63</v>
+      </c>
+      <c r="F2">
+        <v>91</v>
+      </c>
+      <c r="G2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>28</v>
+      </c>
+      <c r="D4">
+        <v>56</v>
+      </c>
+      <c r="E4">
+        <v>87</v>
+      </c>
+      <c r="F4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>70</v>
+      </c>
+      <c r="E5">
+        <v>70</v>
+      </c>
+      <c r="F5">
+        <v>70</v>
+      </c>
+      <c r="G5">
+        <v>99</v>
+      </c>
+      <c r="H5">
+        <v>70</v>
+      </c>
+      <c r="I5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>70</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>34</v>
+      </c>
+      <c r="C10">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transmit Data from the Camera via USB to Excel
</commit_message>
<xml_diff>
--- a/ObjectDetection/ObjectDectecionWithOpenCV/TestData/test.xlsx
+++ b/ObjectDetection/ObjectDectecionWithOpenCV/TestData/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -424,6 +425,147 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>37</v>
+      </c>
+      <c r="B1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>73</v>
+      </c>
+      <c r="E2">
+        <v>72</v>
+      </c>
+      <c r="F2">
+        <v>72</v>
+      </c>
+      <c r="G2">
+        <v>106</v>
+      </c>
+      <c r="H2">
+        <v>107</v>
+      </c>
+      <c r="I2">
+        <v>107</v>
+      </c>
+      <c r="J2">
+        <v>108</v>
+      </c>
+      <c r="K2">
+        <v>140</v>
+      </c>
+      <c r="L2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>73</v>
+      </c>
+      <c r="E4">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>29</v>
+      </c>
+      <c r="G4">
+        <v>66</v>
+      </c>
+      <c r="H4">
+        <v>66</v>
+      </c>
+      <c r="I4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>31</v>
+      </c>
+      <c r="F7">
+        <v>67</v>
+      </c>
+      <c r="G7">
+        <v>67</v>
+      </c>
+      <c r="H7">
+        <v>67</v>
+      </c>
+      <c r="I7">
+        <v>102</v>
+      </c>
+      <c r="J7">
+        <v>102</v>
+      </c>
+      <c r="K7">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>29</v>
+      </c>
+      <c r="G10">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>32</v>
+      </c>
+      <c r="F13">
+        <v>63</v>
+      </c>
+      <c r="G13">
+        <v>63</v>
+      </c>
+      <c r="H13">
+        <v>95</v>
+      </c>
+      <c r="I13">
+        <v>129</v>
+      </c>
+      <c r="J13">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
@@ -703,10 +845,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H8"/>
+  <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,6 +890,17 @@
         <v>71</v>
       </c>
     </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>61</v>
+      </c>
+      <c r="C10">
+        <v>61</v>
+      </c>
+      <c r="E10">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -757,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,8 +980,14 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>56</v>
+      </c>
       <c r="C7">
         <v>70</v>
+      </c>
+      <c r="D7">
+        <v>57</v>
       </c>
       <c r="E7">
         <v>0</v>

</xml_diff>